<commit_message>
Added CSV output support
</commit_message>
<xml_diff>
--- a/AlgoComparisons.xlsx
+++ b/AlgoComparisons.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mutode_research\Mutode2 outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mutode_research\newDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13932801-92B1-4396-95AC-96EE65BD6A84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B866CACC-7224-4E14-8DD5-76B87D29AE19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="382" yWindow="382" windowWidth="18351" windowHeight="9558" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
+    <workbookView xWindow="3058" yWindow="3058" windowWidth="18351" windowHeight="9558" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
   <si>
     <t>ddMin</t>
   </si>
@@ -245,9 +245,6 @@
     <t>0-203</t>
   </si>
   <si>
-    <t>10s 0ms</t>
-  </si>
-  <si>
     <t>0s 813ms</t>
   </si>
   <si>
@@ -372,6 +369,45 @@
   </si>
   <si>
     <t>0,1,2,3,4,5,6,7,8,9,10,11,12,13,220,222,223,224,225,226,227,228,229,230,231,232,233,234,235,236,237,238,239,240,241,242,243,244,245,246,247,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,277,278,279,280,281,282,283,284,285,286,287,288,289,290,291,292,293,294,295,296,297,298,299,300,301,302,303,304,305,306,307,308,309,310,311,312,313,314,315,316,317,318,319,320,321,322,323,324,325,326,327,328,329,330,331,332,333,334,335,336,337,338,339,340,341,342,343,344,345,346,347,348,349,350,351,364,373,374,375,376,377,378,379,380,381,382,383,384,385,386,387,388,389,390,391,392,393,394,395,396,397,398,399,400,401,402,403,404,405,406,407,408,409,410,411,412,413,414,415,416,417,418,419,420,421,422,423,424,425,426</t>
+  </si>
+  <si>
+    <t>Mutode Running Time</t>
+  </si>
+  <si>
+    <t>Mutants Killed2</t>
+  </si>
+  <si>
+    <t>Mutants Generated</t>
+  </si>
+  <si>
+    <t>Mutants Survived</t>
+  </si>
+  <si>
+    <t>Mutants Discarded</t>
+  </si>
+  <si>
+    <t>43m 53s</t>
+  </si>
+  <si>
+    <t>20m 29s</t>
+  </si>
+  <si>
+    <t>20m 13s</t>
+  </si>
+  <si>
+    <t>2h 36m</t>
+  </si>
+  <si>
+    <t>2m 24s</t>
+  </si>
+  <si>
+    <t>14m 48s</t>
+  </si>
+  <si>
+    <t>26m 22s</t>
+  </si>
+  <si>
+    <t>4h 12.9s</t>
   </si>
 </sst>
 </file>
@@ -609,6 +645,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -627,12 +669,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Accent2" xfId="7" builtinId="33"/>
@@ -644,7 +680,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="5" xr:uid="{F4E56029-7EE9-453F-ADCF-12C8305BF6E8}"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="49">
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -662,9 +713,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -672,6 +720,43 @@
           <color theme="4" tint="0.499984740745262"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF9C5700"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -730,40 +815,6 @@
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF9C5700"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -872,75 +923,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{952538F1-7DF3-4D7D-A8CC-BE4F7FA56AC6}" name="Table8" displayName="Table8" ref="G2:M23" totalsRowShown="0" headerRowDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{952538F1-7DF3-4D7D-A8CC-BE4F7FA56AC6}" name="Table8" displayName="Table8" ref="L2:R23" totalsRowShown="0" headerRowDxfId="48" tableBorderDxfId="47" headerRowCellStyle="Explanatory Text">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12B54DEA-7254-4D41-BEC3-BEA4C9B5FD2B}" name="AlgorithmRunningTime" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{C041EDEE-7D1D-40B4-A76F-BE7D7A036172}" name="Reduced Subset" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{2D65E345-C673-4CC1-939C-6D0BF18353C1}" name="Mutation Score" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{4CC4BD8C-4EF4-43AB-BAAB-4E7F5B7FD70D}" name="Coverage" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{644740EE-5F30-46BC-A81B-59EA94F094F2}" name="ReducedTestSuiteRunningTime" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{6C008CB6-3003-451B-83F5-7A2E2094A09F}" name="Tolerance" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{D105531A-8670-4AD8-BDF7-70ED045D32AA}" name="ReducedTestSuiteSize" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{12B54DEA-7254-4D41-BEC3-BEA4C9B5FD2B}" name="AlgorithmRunningTime" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{C041EDEE-7D1D-40B4-A76F-BE7D7A036172}" name="Reduced Subset" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{2D65E345-C673-4CC1-939C-6D0BF18353C1}" name="Mutation Score" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{4CC4BD8C-4EF4-43AB-BAAB-4E7F5B7FD70D}" name="Coverage" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{644740EE-5F30-46BC-A81B-59EA94F094F2}" name="ReducedTestSuiteRunningTime" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{6C008CB6-3003-451B-83F5-7A2E2094A09F}" name="Tolerance" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{D105531A-8670-4AD8-BDF7-70ED045D32AA}" name="ReducedTestSuiteSize" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{14F4EC92-7BFE-403F-A3C6-CD427D010934}" name="Table9" displayName="Table9" ref="N2:T23" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32" headerRowCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{14F4EC92-7BFE-403F-A3C6-CD427D010934}" name="Table9" displayName="Table9" ref="S2:Y23" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37" headerRowCellStyle="Explanatory Text">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6C9C0781-48E2-4FB7-8744-C1EDD4F95DCB}" name="AlgorithmRunningTime" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{DA4A4864-0763-4B71-A651-ED4CA4A414F2}" name="Reduced Subset" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{0303DEB1-3A97-457B-8F0B-075435BD2CA4}" name="Mutation Score" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{37441378-B4C1-4801-8946-B5F26FB1A9B8}" name="Coverage" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{5676F7B9-8FF9-49ED-8633-08C2401FF4B2}" name="ReducedTestSuiteRunningTime" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{7E74752D-6DE1-4C73-B537-CFA8D85EDF85}" name="Tolerance" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{2D9D7CF3-D3B4-464C-B1F1-62F1441FBB67}" name="TestSuite Size" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{6C9C0781-48E2-4FB7-8744-C1EDD4F95DCB}" name="AlgorithmRunningTime" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{DA4A4864-0763-4B71-A651-ED4CA4A414F2}" name="Reduced Subset" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{0303DEB1-3A97-457B-8F0B-075435BD2CA4}" name="Mutation Score" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{37441378-B4C1-4801-8946-B5F26FB1A9B8}" name="Coverage" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{5676F7B9-8FF9-49ED-8633-08C2401FF4B2}" name="ReducedTestSuiteRunningTime" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{7E74752D-6DE1-4C73-B537-CFA8D85EDF85}" name="Tolerance" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{2D9D7CF3-D3B4-464C-B1F1-62F1441FBB67}" name="TestSuite Size" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{21AC0CEF-D177-4D66-B441-7618BEEDE8E3}" name="Table10" displayName="Table10" ref="U2:AD23" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17" headerRowCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{21AC0CEF-D177-4D66-B441-7618BEEDE8E3}" name="Table10" displayName="Table10" ref="Z2:AI23" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28" headerRowCellStyle="Explanatory Text">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9B95FA3B-E111-47B3-9FEB-6E34F77C693F}" name="AlgorithmRunningTime"/>
-    <tableColumn id="2" xr3:uid="{CE31A1F2-CCFB-41B9-802E-E4E7D6C22363}" name="Reduced Subset" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C3588D6B-9C88-46A6-AD70-75921A04F317}" name="Mutation Score" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{640DAF15-6CE5-424F-B23B-0356D0396E43}" name="Coverage" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{72017D7E-EB7B-455E-8490-433A112AD377}" name="ReducedTestSuiteRunningTime" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{2495EE0C-328B-4914-946A-3D5B24547ED9}" name="Starting Tolerance" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{42E4F09C-725B-46FD-8BC3-921A3329D1A6}" name="ToleranceThatFoundASet" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{8E19AD31-C6CB-4914-89F0-9353B6A7CD33}" name="TotalRuns" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{DB462F9A-ABEA-418C-81ED-46797C03550C}" name="ExecutedRuns" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{59135B1B-35D4-4DDB-B9C3-6D510C325029}" name="TestSuite Size" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{CE31A1F2-CCFB-41B9-802E-E4E7D6C22363}" name="Reduced Subset" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{C3588D6B-9C88-46A6-AD70-75921A04F317}" name="Mutation Score" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{640DAF15-6CE5-424F-B23B-0356D0396E43}" name="Coverage" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{72017D7E-EB7B-455E-8490-433A112AD377}" name="ReducedTestSuiteRunningTime" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{2495EE0C-328B-4914-946A-3D5B24547ED9}" name="Starting Tolerance" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{42E4F09C-725B-46FD-8BC3-921A3329D1A6}" name="ToleranceThatFoundASet" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{8E19AD31-C6CB-4914-89F0-9353B6A7CD33}" name="TotalRuns" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{DB462F9A-ABEA-418C-81ED-46797C03550C}" name="ExecutedRuns" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{59135B1B-35D4-4DDB-B9C3-6D510C325029}" name="TestSuite Size" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="B1:F23" totalsRowShown="0" headerRowDxfId="24" headerRowCellStyle="Neutral">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Mutation Score" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{3699F74C-ECE0-4B26-9682-8D573AD734B8}" name="Coverage" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{CD2ECBD2-6A54-4B63-8B16-769F2F08101F}" name="OriginalTestSuiteRunningTime" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{1D29439A-E95C-4EAB-9C6A-44F1FBC75F33}" name="Orignal TestSuite Size" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="B1:K23" totalsRowShown="0" headerRowDxfId="18" headerRowCellStyle="Neutral">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Mutation Score" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{3699F74C-ECE0-4B26-9682-8D573AD734B8}" name="Coverage" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{CD2ECBD2-6A54-4B63-8B16-769F2F08101F}" name="OriginalTestSuiteRunningTime" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{1D29439A-E95C-4EAB-9C6A-44F1FBC75F33}" name="Orignal TestSuite Size" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{1ED35EFA-8CCC-4F74-B0BA-63D0F2B0C067}" name="Mutode Running Time" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{B31DCAD0-6793-4E02-937E-37FDBF007C2A}" name="Mutants Generated" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{1D18328C-BCA6-4FAC-B58B-4BBF7D4449EA}" name="Mutants Killed2" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6EED791C-77AD-4042-BF9C-F7480F2D4091}" name="Mutants Survived" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{B04458F3-7CA1-40EA-8E87-222BB12FE8D9}" name="Mutants Discarded" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0109829-D30D-42C3-9E57-90E25F812D9E}" name="Table2" displayName="Table2" ref="AE2:AJ23" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="7" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0109829-D30D-42C3-9E57-90E25F812D9E}" name="Table2" displayName="Table2" ref="AJ2:AO23" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11" headerRowCellStyle="Accent2">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E4B25968-3AB6-460C-BC4A-98BCD3ED878C}" name="AlgorithmRunningTime" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{3DDDEECD-8312-4190-AA68-6A4E84D065A9}" name="Features to be selected" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{6FD36AEB-1C1B-4058-AE87-EA5A28CA5C75}" name="Reduced Subset" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F3703558-BD53-4188-AEE9-6233EB063F72}" name="Mutation Score" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4D7349A3-5B31-4CC5-A72F-4B706196187A}" name="Coverage" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{ED760C3C-7A39-4043-B686-87F211ABDA26}" name="ReducedTestSuiteRunningTime" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E4B25968-3AB6-460C-BC4A-98BCD3ED878C}" name="AlgorithmRunningTime" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{3DDDEECD-8312-4190-AA68-6A4E84D065A9}" name="Features to be selected" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{6FD36AEB-1C1B-4058-AE87-EA5A28CA5C75}" name="Reduced Subset" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{F3703558-BD53-4188-AEE9-6233EB063F72}" name="Mutation Score" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{4D7349A3-5B31-4CC5-A72F-4B706196187A}" name="Coverage" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{ED760C3C-7A39-4043-B686-87F211ABDA26}" name="ReducedTestSuiteRunningTime" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1243,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A84B95-A035-4AC9-8702-F9EE4E2D8975}">
-  <dimension ref="A1:AJ23"/>
+  <dimension ref="A1:AO23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
@@ -1256,11 +1312,12 @@
     <col min="3" max="3" width="19.21875" style="6" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" style="6" customWidth="1"/>
     <col min="5" max="5" width="33.44140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="19.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="26" style="6" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="29.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="6" customWidth="1"/>
     <col min="12" max="12" width="20.21875" style="6" customWidth="1"/>
     <col min="13" max="13" width="16.5546875" style="6" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" style="6" customWidth="1"/>
@@ -1285,8 +1342,8 @@
     <col min="36" max="36" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" ht="36.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:41" s="3" customFormat="1" ht="36.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1304,144 +1361,164 @@
       <c r="F1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16" t="s">
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="17" t="s">
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
+      <c r="AN1" s="20"/>
+      <c r="AO1" s="20"/>
     </row>
-    <row r="2" spans="1:36" s="1" customFormat="1" ht="20.399999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
+    <row r="2" spans="1:41" s="1" customFormat="1" ht="20.399999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="AC2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AD2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AF2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AG2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AH2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AI2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" s="19" t="s">
+      <c r="AJ2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AK2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AM2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AN2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AO2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1461,97 +1538,112 @@
         <v>17</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2891</v>
+      </c>
+      <c r="I3" s="6">
+        <v>2655</v>
+      </c>
+      <c r="J3" s="6">
+        <v>208</v>
+      </c>
+      <c r="K3" s="6">
+        <v>28</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="9">
+      <c r="N3" s="9">
         <v>0.85160000000000002</v>
       </c>
-      <c r="J3" s="9">
+      <c r="O3" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="6">
-        <v>10</v>
-      </c>
-      <c r="M3" s="6">
+      <c r="Q3" s="6">
+        <v>10</v>
+      </c>
+      <c r="R3" s="6">
         <v>2</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="9">
+      <c r="U3" s="9">
         <v>0.85160000000000002</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="V3" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="10">
-        <v>10</v>
-      </c>
-      <c r="T3" s="10">
+      <c r="X3" s="10">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="10">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Z3" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>10</v>
       </c>
       <c r="AD3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AE3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK3" s="6">
+        <v>8</v>
+      </c>
+      <c r="AL3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="AF3" s="6">
-        <v>8</v>
-      </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AM3" s="9">
+        <v>0.92559999999999998</v>
+      </c>
+      <c r="AN3" s="9">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="AO3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="AH3" s="9">
-        <v>0.92559999999999998</v>
-      </c>
-      <c r="AI3" s="9">
-        <v>0.91410000000000002</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>101</v>
-      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1571,97 +1663,112 @@
         <v>4</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1300</v>
+      </c>
+      <c r="I4" s="6">
+        <v>106</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1189</v>
+      </c>
+      <c r="K4" s="6">
+        <v>5</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="6">
+      <c r="M4" s="6">
         <v>3</v>
       </c>
-      <c r="I4" s="9">
+      <c r="N4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="J4" s="9">
+      <c r="O4" s="9">
         <v>0.43330000000000002</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="6">
-        <v>10</v>
-      </c>
-      <c r="M4" s="6">
+      <c r="Q4" s="6">
+        <v>10</v>
+      </c>
+      <c r="R4" s="6">
         <v>1</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="6">
+      <c r="T4" s="6">
         <v>3</v>
       </c>
-      <c r="P4" s="9">
+      <c r="U4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="V4" s="9">
         <v>0.69610000000000005</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="W4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="10">
+      <c r="X4" s="10">
         <v>1</v>
       </c>
-      <c r="T4" s="10">
+      <c r="Y4" s="10">
         <v>1</v>
       </c>
-      <c r="U4" t="s">
+      <c r="Z4" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="6">
+      <c r="AA4" s="6">
         <v>0</v>
       </c>
-      <c r="W4" s="11">
+      <c r="AB4" s="11">
         <v>0</v>
       </c>
-      <c r="X4" s="9">
+      <c r="AC4" s="9">
         <v>0.48070000000000002</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="AD4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="AE4" s="6">
         <v>1</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AF4" s="6">
         <v>3.68</v>
       </c>
-      <c r="AB4" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC4" s="6">
+      <c r="AG4" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH4" s="6">
         <v>2</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="AI4" s="6">
         <v>1</v>
       </c>
-      <c r="AE4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF4" s="6">
+      <c r="AJ4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK4" s="6">
         <v>2</v>
       </c>
-      <c r="AG4" s="6" t="s">
+      <c r="AL4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM4" s="9">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="AN4" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="AO4" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="AH4" s="9">
-        <v>3.6799999999999999E-2</v>
-      </c>
-      <c r="AI4" s="11">
-        <v>0.68</v>
-      </c>
-      <c r="AJ4" s="11" t="s">
-        <v>95</v>
-      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1681,97 +1788,112 @@
         <v>218</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="6">
+        <v>976</v>
+      </c>
+      <c r="I5" s="6">
+        <v>766</v>
+      </c>
+      <c r="J5" s="6">
+        <v>175</v>
+      </c>
+      <c r="K5" s="6">
+        <v>35</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="9">
+      <c r="N5" s="9">
         <v>0.64529999999999998</v>
       </c>
-      <c r="J5" s="9">
+      <c r="O5" s="9">
         <v>0.88549999999999995</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="6">
-        <v>10</v>
-      </c>
-      <c r="M5" s="6">
+      <c r="Q5" s="6">
+        <v>10</v>
+      </c>
+      <c r="R5" s="6">
         <v>42</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="9">
+      <c r="U5" s="9">
         <v>0.64529999999999998</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="V5" s="9">
         <v>0.89159999999999995</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="10">
-        <v>10</v>
-      </c>
-      <c r="T5" s="10">
+      <c r="X5" s="10">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="10">
         <v>40</v>
       </c>
-      <c r="U5" t="s">
+      <c r="Z5" t="s">
         <v>49</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="AA5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="AB5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="AC5" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z5" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB5" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC5" s="6">
-        <v>10</v>
       </c>
       <c r="AD5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AE5" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF5" s="6">
+      <c r="AE5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK5" s="6">
         <v>109</v>
       </c>
-      <c r="AG5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH5" s="9">
+      <c r="AL5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM5" s="9">
         <v>0.47149999999999997</v>
       </c>
-      <c r="AI5" s="9">
+      <c r="AN5" s="9">
         <v>0.86729999999999996</v>
       </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AO5" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1791,102 +1913,117 @@
         <v>858</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3900</v>
+      </c>
+      <c r="I6" s="6">
+        <v>2900</v>
+      </c>
+      <c r="J6" s="6">
+        <v>607</v>
+      </c>
+      <c r="K6" s="6">
+        <v>393</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="9">
+      <c r="N6" s="9">
         <v>0.63239999999999996</v>
       </c>
-      <c r="J6" s="9">
+      <c r="O6" s="9">
         <v>0.82330000000000003</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="6">
-        <v>10</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="Q6" s="6">
+        <v>10</v>
+      </c>
+      <c r="R6" s="6">
         <v>156</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="9">
+      <c r="U6" s="9">
         <v>0.63239999999999996</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="V6" s="9">
         <v>0.85670000000000002</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="W6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="10">
-        <v>10</v>
-      </c>
-      <c r="T6" s="10">
+      <c r="X6" s="10">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="10">
         <v>144</v>
       </c>
-      <c r="U6" t="s">
+      <c r="Z6" t="s">
         <v>50</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="AA6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="AB6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X6" s="6" t="s">
+      <c r="AC6" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z6" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB6" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC6" s="6">
-        <v>10</v>
       </c>
       <c r="AD6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AE6" s="6" t="s">
+      <c r="AE6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK6" s="6">
+        <v>200</v>
+      </c>
+      <c r="AL6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AF6" s="6">
-        <v>200</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH6" s="9">
+      <c r="AM6" s="9">
         <v>0.29409999999999997</v>
       </c>
-      <c r="AI6" s="9">
+      <c r="AN6" s="9">
         <v>0.71609999999999996</v>
       </c>
-      <c r="AJ6" s="6" t="s">
-        <v>73</v>
+      <c r="AO6" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="C7" s="11">
         <v>0</v>
@@ -1895,103 +2032,118 @@
         <v>0.81159999999999999</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="6">
         <v>8</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="6">
+        <v>70</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" s="6">
+        <v>65</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="6">
+        <v>7</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0.79710000000000003</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="6">
+      <c r="Q7" s="6">
+        <v>10</v>
+      </c>
+      <c r="R7" s="6">
+        <v>1</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="U7" s="11">
+        <v>0</v>
+      </c>
+      <c r="V7" s="11">
+        <v>0</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="X7" s="10">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB7" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="9">
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>10</v>
+      </c>
+      <c r="AF7" s="11">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="6">
         <v>7</v>
       </c>
-      <c r="I7" s="11">
+      <c r="AJ7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK7" s="6">
+        <v>4</v>
+      </c>
+      <c r="AL7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM7" s="11">
         <v>0</v>
       </c>
-      <c r="J7" s="9">
-        <v>0.79710000000000003</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L7" s="6">
-        <v>10</v>
-      </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>0</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="10">
-        <v>10</v>
-      </c>
-      <c r="T7" s="10">
-        <v>0</v>
-      </c>
-      <c r="U7" t="s">
-        <v>81</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="W7" s="11">
-        <v>0</v>
-      </c>
-      <c r="X7" s="9">
-        <v>0.81159999999999999</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="6">
-        <v>7</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF7" s="6">
-        <v>4</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="9">
+      <c r="AN7" s="9">
         <v>0.57450000000000001</v>
       </c>
-      <c r="AJ7" s="6" t="s">
-        <v>95</v>
+      <c r="AO7" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2011,97 +2163,112 @@
         <v>3</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="6">
+        <v>814</v>
+      </c>
+      <c r="I8" s="6">
+        <v>94</v>
+      </c>
+      <c r="J8" s="6">
+        <v>717</v>
+      </c>
+      <c r="K8" s="6">
+        <v>3</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="6">
+      <c r="M8" s="6">
         <v>2</v>
       </c>
-      <c r="I8" s="9">
+      <c r="N8" s="9">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="J8" s="9">
+      <c r="O8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="P8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="6">
-        <v>10</v>
-      </c>
-      <c r="M8" s="6">
+      <c r="Q8" s="6">
+        <v>10</v>
+      </c>
+      <c r="R8" s="6">
         <v>1</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="6">
+      <c r="T8" s="6">
         <v>2</v>
       </c>
-      <c r="P8" s="9">
+      <c r="U8" s="9">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="V8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="W8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="S8" s="10">
+      <c r="X8" s="10">
         <v>1</v>
       </c>
-      <c r="T8" s="10">
+      <c r="Y8" s="10">
         <v>1</v>
       </c>
-      <c r="U8" t="s">
+      <c r="Z8" t="s">
         <v>63</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="AA8" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="11">
+      <c r="AB8" s="11">
         <v>0</v>
       </c>
-      <c r="X8" s="11">
+      <c r="AC8" s="11">
         <v>0</v>
       </c>
-      <c r="Y8" s="6" t="s">
+      <c r="AD8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="AE8" s="6">
         <v>1</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AF8" s="6">
         <v>5.88</v>
       </c>
-      <c r="AB8" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC8" s="6">
+      <c r="AG8" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH8" s="6">
         <v>2</v>
       </c>
-      <c r="AD8" s="6">
+      <c r="AI8" s="6">
         <v>0</v>
       </c>
-      <c r="AE8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF8" s="6">
+      <c r="AJ8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK8" s="6">
         <v>1</v>
       </c>
-      <c r="AG8" s="6">
+      <c r="AL8" s="6">
         <v>2</v>
       </c>
-      <c r="AH8" s="9">
+      <c r="AM8" s="9">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="AI8" s="9">
+      <c r="AN8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="AJ8" s="6" t="s">
-        <v>96</v>
+      <c r="AO8" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -2115,108 +2282,123 @@
         <v>1</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="F9" s="6">
         <v>204</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="6">
+        <v>885</v>
+      </c>
+      <c r="I9" s="6">
+        <v>701</v>
+      </c>
+      <c r="J9" s="6">
+        <v>157</v>
+      </c>
+      <c r="K9" s="6">
+        <v>27</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="N9" s="9">
+        <v>0.6744</v>
+      </c>
+      <c r="O9" s="9">
+        <v>0.89339999999999997</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>10</v>
+      </c>
+      <c r="R9" s="6">
+        <v>42</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="9">
+      <c r="U9" s="9">
         <v>0.6744</v>
       </c>
-      <c r="J9" s="9">
-        <v>0.89339999999999997</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="6">
-        <v>10</v>
-      </c>
-      <c r="M9" s="6">
-        <v>42</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="V9" s="9">
+        <v>0.89659999999999995</v>
+      </c>
+      <c r="W9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="P9" s="9">
-        <v>0.6744</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>0.89659999999999995</v>
-      </c>
-      <c r="R9" s="6" t="s">
+      <c r="X9" s="10">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>35</v>
+      </c>
+      <c r="Z9" t="s">
         <v>73</v>
       </c>
-      <c r="S9" s="10">
-        <v>10</v>
-      </c>
-      <c r="T9" s="10">
-        <v>35</v>
-      </c>
-      <c r="U9" t="s">
-        <v>74</v>
-      </c>
-      <c r="V9" s="6" t="s">
+      <c r="AA9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="AB9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X9" s="6" t="s">
+      <c r="AC9" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z9" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB9" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC9" s="6">
-        <v>10</v>
       </c>
       <c r="AD9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AE9" s="6" t="s">
+      <c r="AE9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AI9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK9" s="6">
+        <v>102</v>
+      </c>
+      <c r="AL9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM9" s="9">
+        <v>0.47120000000000001</v>
+      </c>
+      <c r="AN9" s="9">
+        <v>0.879</v>
+      </c>
+      <c r="AO9" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AF9" s="6">
-        <v>102</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH9" s="9">
-        <v>0.47120000000000001</v>
-      </c>
-      <c r="AI9" s="9">
-        <v>0.879</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>104</v>
-      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="9">
         <v>0.76190000000000002</v>
@@ -2225,108 +2407,123 @@
         <v>0.98660000000000003</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="6">
         <v>833</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="6">
+        <v>3788</v>
+      </c>
+      <c r="I10" s="6">
+        <v>2713</v>
+      </c>
+      <c r="J10" s="6">
+        <v>698</v>
+      </c>
+      <c r="K10" s="6">
+        <v>377</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="N10" s="9">
+        <v>0.66190000000000004</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0.81289999999999996</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>10</v>
+      </c>
+      <c r="R10" s="6">
+        <v>148</v>
+      </c>
+      <c r="S10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="9">
+      <c r="T10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="U10" s="9">
         <v>0.66190000000000004</v>
       </c>
-      <c r="J10" s="9">
-        <v>0.81289999999999996</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" s="6">
-        <v>10</v>
-      </c>
-      <c r="M10" s="6">
-        <v>148</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="O10" s="6" t="s">
+      <c r="V10" s="9">
+        <v>0.84930000000000005</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="X10" s="10">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>129</v>
+      </c>
+      <c r="Z10" t="s">
         <v>90</v>
       </c>
-      <c r="P10" s="9">
-        <v>0.66190000000000004</v>
-      </c>
-      <c r="Q10" s="9">
-        <v>0.84930000000000005</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="S10" s="10">
-        <v>10</v>
-      </c>
-      <c r="T10" s="10">
-        <v>129</v>
-      </c>
-      <c r="U10" t="s">
-        <v>91</v>
-      </c>
-      <c r="V10" s="6" t="s">
+      <c r="AA10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W10" s="6" t="s">
+      <c r="AB10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X10" s="6" t="s">
+      <c r="AC10" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z10" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>10</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>10</v>
       </c>
       <c r="AD10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AE10" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF10" s="6">
+      <c r="AE10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AF10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK10" s="6">
         <v>200</v>
       </c>
-      <c r="AG10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH10" s="9">
+      <c r="AL10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM10" s="9">
         <v>0.35859999999999997</v>
       </c>
-      <c r="AI10" s="9">
+      <c r="AN10" s="9">
         <v>0.70920000000000005</v>
       </c>
-      <c r="AJ10" s="6" t="s">
+      <c r="AO10" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
@@ -2337,13 +2534,18 @@
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
@@ -2354,13 +2556,18 @@
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
       <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
@@ -2371,13 +2578,18 @@
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
       <c r="AJ13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
@@ -2388,13 +2600,18 @@
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
       <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15"/>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
@@ -2405,13 +2622,18 @@
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="6"/>
+      <c r="AN15" s="6"/>
+      <c r="AO15" s="6"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
@@ -2422,13 +2644,18 @@
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="6"/>
+      <c r="AK16" s="6"/>
+      <c r="AL16" s="6"/>
+      <c r="AM16" s="6"/>
+      <c r="AN16" s="6"/>
+      <c r="AO16" s="6"/>
     </row>
-    <row r="17" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17"/>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
@@ -2439,13 +2666,18 @@
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
+      <c r="AM17" s="6"/>
+      <c r="AN17" s="6"/>
+      <c r="AO17" s="6"/>
     </row>
-    <row r="18" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
@@ -2456,13 +2688,18 @@
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="6"/>
+      <c r="AK18" s="6"/>
+      <c r="AL18" s="6"/>
+      <c r="AM18" s="6"/>
+      <c r="AN18" s="6"/>
+      <c r="AO18" s="6"/>
     </row>
-    <row r="19" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19"/>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
@@ -2473,13 +2710,18 @@
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="6"/>
+      <c r="AK19" s="6"/>
+      <c r="AL19" s="6"/>
+      <c r="AM19" s="6"/>
+      <c r="AN19" s="6"/>
+      <c r="AO19" s="6"/>
     </row>
-    <row r="20" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20"/>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
@@ -2490,13 +2732,18 @@
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="6"/>
+      <c r="AK20" s="6"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="6"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="6"/>
     </row>
-    <row r="21" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
@@ -2507,13 +2754,18 @@
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="6"/>
+      <c r="AK21" s="6"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
@@ -2524,13 +2776,18 @@
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="6"/>
+      <c r="AK22" s="6"/>
+      <c r="AL22" s="6"/>
+      <c r="AM22" s="6"/>
+      <c r="AN22" s="6"/>
+      <c r="AO22" s="6"/>
     </row>
-    <row r="23" spans="17:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="17:41" x14ac:dyDescent="0.3">
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
@@ -2541,14 +2798,19 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="6"/>
+      <c r="AK23" s="6"/>
+      <c r="AL23" s="6"/>
+      <c r="AM23" s="6"/>
+      <c r="AN23" s="6"/>
+      <c r="AO23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="G1:M1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="U1:AD1"/>
-    <mergeCell ref="AE1:AJ1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AI1"/>
+    <mergeCell ref="AJ1:AO1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>

</xml_diff>